<commit_message>
fix usb connector issue
</commit_message>
<xml_diff>
--- a/pcb/elflet-bom.xlsx
+++ b/pcb/elflet-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="20" windowWidth="25620" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="125">
   <si>
     <t>Attribute</t>
     <phoneticPr fontId="1"/>
@@ -240,14 +240,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>C1, C2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">3216/2uF/50V(10%) </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <t>1608/</t>
     </r>
@@ -485,14 +477,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>GRM31MB11H224KA01L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>http://akizukidenshi.com/catalog/g/gP-09323/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>GRM188B11E104KA01</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -788,6 +772,38 @@
   </si>
   <si>
     <t>http://akizukidenshi.com/catalog/g/gC-09717/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ECJ(L(3))FF1E105Z</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://akizukidenshi.com/catalog/g/gP-08708/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3216/1uF/25V(+80-20%) </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GRM31MF11C475ZA01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3216/4.7uF/16V(+80-20%)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://akizukidenshi.com/catalog/g/gP-04661/</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -893,7 +909,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -914,13 +930,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1255,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1273,8 +1292,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28">
-      <c r="A1" s="9" t="s">
-        <v>105</v>
+      <c r="A1" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1291,10 +1310,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1310,8 +1329,8 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>81</v>
+      <c r="E3" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>40</v>
@@ -1330,9 +1349,9 @@
       <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1348,9 +1367,9 @@
       <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1370,7 +1389,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1387,10 +1406,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1407,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>20</v>
@@ -1426,11 +1445,11 @@
       <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>84</v>
+      <c r="E9" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1446,9 +1465,9 @@
       <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1459,14 +1478,14 @@
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1474,7 +1493,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>33</v>
@@ -1482,7 +1501,7 @@
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1491,16 +1510,16 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="3"/>
@@ -1518,8 +1537,8 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>82</v>
+      <c r="E14" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>39</v>
@@ -1527,279 +1546,281 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
-      </c>
-      <c r="E15" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="5" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="3">
-        <v>4</v>
-      </c>
-      <c r="E16" s="6"/>
+      <c r="A16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="5" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D17" s="3">
-        <v>2</v>
-      </c>
-      <c r="E17" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="10"/>
       <c r="F17" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3">
-        <v>6</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>85</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="5" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="F20" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="5" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="5" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="10"/>
       <c r="F25" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28">
-      <c r="A29" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2" t="s">
+    </row>
+    <row r="30" spans="1:6" ht="28">
+      <c r="A30" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>118</v>
+      <c r="E31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1808,39 +1829,55 @@
         <v>110</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="9"/>
       <c r="F33" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D34" s="3">
         <v>1</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F34" s="3"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E9:E12"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="E20:E27"/>
+    <mergeCell ref="E32:E34"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -1848,8 +1885,8 @@
     <hyperlink ref="F12" r:id="rId2"/>
     <hyperlink ref="F14" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F21" r:id="rId5"/>
-    <hyperlink ref="F26" r:id="rId6"/>
+    <hyperlink ref="F22" r:id="rId5"/>
+    <hyperlink ref="F27" r:id="rId6"/>
     <hyperlink ref="F4" r:id="rId7"/>
     <hyperlink ref="F5" r:id="rId8"/>
     <hyperlink ref="F7" r:id="rId9"/>
@@ -1857,19 +1894,20 @@
     <hyperlink ref="F10" r:id="rId11"/>
     <hyperlink ref="F11" r:id="rId12"/>
     <hyperlink ref="F15" r:id="rId13"/>
-    <hyperlink ref="F16" r:id="rId14"/>
-    <hyperlink ref="F17" r:id="rId15"/>
-    <hyperlink ref="F18" r:id="rId16"/>
-    <hyperlink ref="F22" r:id="rId17"/>
-    <hyperlink ref="F19" r:id="rId18"/>
-    <hyperlink ref="F20" r:id="rId19"/>
-    <hyperlink ref="F23" r:id="rId20"/>
-    <hyperlink ref="F24" r:id="rId21"/>
-    <hyperlink ref="F25" r:id="rId22"/>
+    <hyperlink ref="F17" r:id="rId14"/>
+    <hyperlink ref="F18" r:id="rId15"/>
+    <hyperlink ref="F19" r:id="rId16"/>
+    <hyperlink ref="F23" r:id="rId17"/>
+    <hyperlink ref="F20" r:id="rId18"/>
+    <hyperlink ref="F21" r:id="rId19"/>
+    <hyperlink ref="F24" r:id="rId20"/>
+    <hyperlink ref="F25" r:id="rId21"/>
+    <hyperlink ref="F26" r:id="rId22"/>
     <hyperlink ref="F6" r:id="rId23"/>
-    <hyperlink ref="F32" r:id="rId24"/>
-    <hyperlink ref="F31" r:id="rId25"/>
-    <hyperlink ref="F33" r:id="rId26"/>
+    <hyperlink ref="F33" r:id="rId24"/>
+    <hyperlink ref="F32" r:id="rId25"/>
+    <hyperlink ref="F34" r:id="rId26"/>
+    <hyperlink ref="F16" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>